<commit_message>
All summary stats updated
</commit_message>
<xml_diff>
--- a/data-files/LL_84_data_files/LL84_building_summary_statistics.xlsx
+++ b/data-files/LL_84_data_files/LL84_building_summary_statistics.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://envienstudio.sharepoint.com/Shared Documents/Potential/DOE R&amp;D Submission/3 - Market Research/targetMarket/data-files/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://envienstudio.sharepoint.com/Shared Documents/Potential/DOE R&amp;D Submission/3 - Market Research/targetMarket/data-files/LL_84_data_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="14_{B99FADF5-1198-41A6-8681-F76E6AAB9B1D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{04C32C9A-749B-4449-AD16-108F594CD9B9}"/>
+  <xr:revisionPtr revIDLastSave="4" documentId="14_{B99FADF5-1198-41A6-8681-F76E6AAB9B1D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{10A3643B-A79E-4376-8FC6-B73FB4E8FECE}"/>
   <bookViews>
-    <workbookView xWindow="13965" yWindow="-16320" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary with Graphs" sheetId="1" r:id="rId1"/>
@@ -757,11 +757,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:G73"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="22" customWidth="1"/>
+    <col min="6" max="6" width="23.140625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
@@ -2451,8 +2455,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:K73"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11254,15 +11258,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101005983132403D1464F8DDC272820BA8C1B" ma:contentTypeVersion="17" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="6fe6f55e11da51139aa85f6a00701c7d">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="d4fe9914-c092-4200-a7d8-cc85a6bef288" xmlns:ns3="afc29c3b-9522-4360-ba9d-c1dc5ac90a19" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="285f550d8d1fc9956465dc5fad4d328f" ns2:_="" ns3:_="">
     <xsd:import namespace="d4fe9914-c092-4200-a7d8-cc85a6bef288"/>
@@ -11511,6 +11506,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4C487A96-5D69-4E40-93EA-4CE92A19EF23}">
   <ds:schemaRefs>
@@ -11523,14 +11527,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AC22D0B1-3E94-4CEC-995E-8A27B9DA16AA}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{72C4F955-2A09-42F6-A5D3-D01882DC6FB3}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -11547,4 +11543,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AC22D0B1-3E94-4CEC-995E-8A27B9DA16AA}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
changed size of LL84 graphic
</commit_message>
<xml_diff>
--- a/data-files/LL_84_data_files/LL84_building_summary_statistics.xlsx
+++ b/data-files/LL_84_data_files/LL84_building_summary_statistics.xlsx
@@ -148,7 +148,7 @@
       <row>1</row>
       <rowOff>0</rowOff>
     </from>
-    <ext cx="17145000" cy="7620000"/>
+    <ext cx="17145000" cy="5715000"/>
     <pic>
       <nvPicPr>
         <cNvPr id="1" name="Image 1" descr="Picture"/>
@@ -9173,13 +9173,13 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{51293A50-F22B-4107-B0F0-8A4F26EEC29F}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2E25A7D6-A606-4A8D-BAC7-3B441E282EB6}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C8A2DF3A-A75D-4572-B045-44CF8349D04D}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1B40D54C-FA44-4D16-9815-38CFA72C0E6B}"/>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D84D6B50-D680-4903-BF3C-8843B8AC5620}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F4BB1C33-48FD-44BD-B56E-9B59215976DE}"/>
 </file>
</xml_diff>